<commit_message>
feat(owners): implement owners module scaffold and feb 24 daily audit
</commit_message>
<xml_diff>
--- a/configs/table-configs/alerts.xlsx
+++ b/configs/table-configs/alerts.xlsx
@@ -403,8 +403,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="35.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -455,7 +467,6 @@
         <v/>
       </c>
       <c r="F2" t="str">
-        <f>IF(SUM($C$2:C2)&lt;=350,"P1",IF(SUM($C$2:C2)&lt;=780,"P2",IF(SUM($C$2:C2)&lt;=1140,"P3",IF(SUM($C$2:C2)&lt;=1880,"P4","P5"))))</f>
         <v>P1</v>
       </c>
       <c r="G2" t="str">
@@ -488,7 +499,6 @@
         <v/>
       </c>
       <c r="F3" t="str">
-        <f>IF(SUM($C$2:C3)&lt;=350,"P1",IF(SUM($C$2:C3)&lt;=780,"P2",IF(SUM($C$2:C3)&lt;=1140,"P3",IF(SUM($C$2:C3)&lt;=1880,"P4","P5"))))</f>
         <v>P1</v>
       </c>
       <c r="G3" t="str">
@@ -521,7 +531,6 @@
         <v>center</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(SUM($C$2:C4)&lt;=350,"P1",IF(SUM($C$2:C4)&lt;=780,"P2",IF(SUM($C$2:C4)&lt;=1140,"P3",IF(SUM($C$2:C4)&lt;=1880,"P4","P5"))))</f>
         <v>P1</v>
       </c>
       <c r="G4" t="str">
@@ -554,7 +563,6 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <f>IF(SUM($C$2:C5)&lt;=350,"P1",IF(SUM($C$2:C5)&lt;=780,"P2",IF(SUM($C$2:C5)&lt;=1140,"P3",IF(SUM($C$2:C5)&lt;=1880,"P4","P5"))))</f>
         <v>P2</v>
       </c>
       <c r="G5" t="str">
@@ -587,7 +595,6 @@
         <v>center</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(SUM($C$2:C6)&lt;=350,"P1",IF(SUM($C$2:C6)&lt;=780,"P2",IF(SUM($C$2:C6)&lt;=1140,"P3",IF(SUM($C$2:C6)&lt;=1880,"P4","P5"))))</f>
         <v>P2</v>
       </c>
       <c r="G6" t="str">
@@ -620,7 +627,6 @@
         <v>center</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(SUM($C$2:C7)&lt;=350,"P1",IF(SUM($C$2:C7)&lt;=780,"P2",IF(SUM($C$2:C7)&lt;=1140,"P3",IF(SUM($C$2:C7)&lt;=1880,"P4","P5"))))</f>
         <v>P3</v>
       </c>
       <c r="G7" t="str">
@@ -653,7 +659,6 @@
         <v/>
       </c>
       <c r="F8" t="str">
-        <f>IF(SUM($C$2:C8)&lt;=350,"P1",IF(SUM($C$2:C8)&lt;=780,"P2",IF(SUM($C$2:C8)&lt;=1140,"P3",IF(SUM($C$2:C8)&lt;=1880,"P4","P5"))))</f>
         <v>P3</v>
       </c>
       <c r="G8" t="str">
@@ -680,8 +685,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -774,8 +783,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -832,8 +846,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -948,8 +969,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="100.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">

</xml_diff>